<commit_message>
Funcionalidades completadas etapa 3
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/structures/Structures.xlsx
+++ b/src/main/resources/reports/structures/Structures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS DOCUMENTOS\CIADTI\PROYECTOS\SERVICIOS\CARGA TRABAJO\ciadti-especifico-carga-trabajo-services\src\main\resources\reports\structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD828E72-2F31-4EA0-BDCE-0678156B9C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921F2167-B2D2-435F-B005-3076D777CEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
   </bookViews>
@@ -1324,7 +1324,7 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG6" sqref="AG6"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1401,7 +1401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:10" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" s="5" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>10</v>
       </c>

</xml_diff>